<commit_message>
Se ajusta lectura de Excel
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Projects\SemilleroSQA\RetoExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Projects\SemilleroSQA\RetoDemoQA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4AC6A8-D506-49E2-A46F-FD54F2197658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE7D6BF-EDE1-4E51-B16A-2CB4245943F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27555" yWindow="5490" windowWidth="15375" windowHeight="7875" xr2:uid="{36E80504-A185-4701-AB87-99BFE8A79D33}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{36E80504-A185-4701-AB87-99BFE8A79D33}"/>
   </bookViews>
   <sheets>
     <sheet name="DataRegister" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Restrepo</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Brahian</t>
+  </si>
+  <si>
+    <t>27 Mar 1997</t>
   </si>
 </sst>
 </file>
@@ -407,13 +410,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7E58C3-97DE-4F87-B93F-E7EF5FF16CD5}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -427,15 +432,18 @@
         <v>5896521456</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>